<commit_message>
Passing first Unit Test
</commit_message>
<xml_diff>
--- a/Domain_Model.xlsx
+++ b/Domain_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vytisvadoklis/Desktop/Airport/airport_challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23948F32-6BD8-E548-B2B7-D7C1878B8B69}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2756FF-FF10-394B-924F-5D040B483770}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18460" yWindow="460" windowWidth="10340" windowHeight="16460" xr2:uid="{FFB222A4-2129-A144-8C04-1D972EFE2B18}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Objects</t>
   </si>
@@ -57,7 +57,10 @@
     <t>prevent_takeoff_when_stormy; prevent_landing_when_stormy; prevent_landing_when_full; let_takeoff; let_landing</t>
   </si>
   <si>
-    <t xml:space="preserve">land; message_grounded_in_the_airport; takeoff; message_left_the_airport; </t>
+    <t xml:space="preserve">land; status_grounded_in_the_airport; takeoff; status_left_the_airport; </t>
+  </si>
+  <si>
+    <t>Variable and default capacity</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,7 +527,9 @@
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Launching plane, checking status
</commit_message>
<xml_diff>
--- a/Domain_Model.xlsx
+++ b/Domain_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vytisvadoklis/Desktop/Airport/airport_challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2756FF-FF10-394B-924F-5D040B483770}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F83B1E9-44AB-9849-B8A0-06D8AF49C1B3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18460" yWindow="460" windowWidth="10340" windowHeight="16460" xr2:uid="{FFB222A4-2129-A144-8C04-1D972EFE2B18}"/>
   </bookViews>
@@ -57,10 +57,10 @@
     <t>prevent_takeoff_when_stormy; prevent_landing_when_stormy; prevent_landing_when_full; let_takeoff; let_landing</t>
   </si>
   <si>
-    <t xml:space="preserve">land; status_grounded_in_the_airport; takeoff; status_left_the_airport; </t>
-  </si>
-  <si>
     <t>Variable and default capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">land; status_grounded?; takeoff; status_flying?; </t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,7 +486,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="64" x14ac:dyDescent="0.2">
@@ -528,7 +528,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Further feature and unit testing - Objects
</commit_message>
<xml_diff>
--- a/Domain_Model.xlsx
+++ b/Domain_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vytisvadoklis/Desktop/Airport/airport_challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F83B1E9-44AB-9849-B8A0-06D8AF49C1B3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCF6F49-0340-2A4C-9408-1330993FF67F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18460" yWindow="460" windowWidth="10340" windowHeight="16460" xr2:uid="{FFB222A4-2129-A144-8C04-1D972EFE2B18}"/>
+    <workbookView xWindow="18720" yWindow="460" windowWidth="10080" windowHeight="16460" xr2:uid="{FFB222A4-2129-A144-8C04-1D972EFE2B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
     <t xml:space="preserve">Messages </t>
   </si>
   <si>
-    <t>sunny; stormy</t>
-  </si>
-  <si>
     <t xml:space="preserve">Air_traffic_controller </t>
   </si>
   <si>
@@ -54,13 +51,16 @@
     <t>System designer</t>
   </si>
   <si>
-    <t>prevent_takeoff_when_stormy; prevent_landing_when_stormy; prevent_landing_when_full; let_takeoff; let_landing</t>
-  </si>
-  <si>
     <t>Variable and default capacity</t>
   </si>
   <si>
-    <t xml:space="preserve">land; status_grounded?; takeoff; status_flying?; </t>
+    <t>prevent_takeoff_when_stormy; prevent_landing_when_stormy; prevent_landing_when_full; let_takeoff; let_landing; plane_in_airport?</t>
+  </si>
+  <si>
+    <t>status_grounded?;</t>
+  </si>
+  <si>
+    <t>sunny; stormy;</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,29 +469,29 @@
     </row>
     <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -519,16 +519,16 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature test pic, change of AR.md and Domain_model
</commit_message>
<xml_diff>
--- a/Domain_Model.xlsx
+++ b/Domain_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vytisvadoklis/Desktop/Airport/airport_challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCF6F49-0340-2A4C-9408-1330993FF67F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41910C77-E425-DA40-9A04-D69EEC319B49}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18720" yWindow="460" windowWidth="10080" windowHeight="16460" xr2:uid="{FFB222A4-2129-A144-8C04-1D972EFE2B18}"/>
   </bookViews>
@@ -450,7 +450,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Step with instance variables complete, other steps  put on hold
</commit_message>
<xml_diff>
--- a/Domain_Model.xlsx
+++ b/Domain_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vytisvadoklis/Desktop/Airport/airport_challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41910C77-E425-DA40-9A04-D69EEC319B49}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A28F20-ED7D-A048-BED3-A447BEDC1E93}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18720" yWindow="460" windowWidth="10080" windowHeight="16460" xr2:uid="{FFB222A4-2129-A144-8C04-1D972EFE2B18}"/>
+    <workbookView xWindow="18720" yWindow="460" windowWidth="15420" windowHeight="16460" xr2:uid="{FFB222A4-2129-A144-8C04-1D972EFE2B18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Objects</t>
   </si>
@@ -51,9 +51,6 @@
     <t>System designer</t>
   </si>
   <si>
-    <t>Variable and default capacity</t>
-  </si>
-  <si>
     <t>prevent_takeoff_when_stormy; prevent_landing_when_stormy; prevent_landing_when_full; let_takeoff; let_landing; plane_in_airport?</t>
   </si>
   <si>
@@ -61,6 +58,12 @@
   </si>
   <si>
     <t>sunny; stormy;</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>no message, but creation of functionality -  variable and default capacity</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -478,7 +481,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -486,7 +489,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="64" x14ac:dyDescent="0.2">
@@ -494,7 +497,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -521,14 +524,16 @@
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>